<commit_message>
Update Entrada.xlsx with new data
</commit_message>
<xml_diff>
--- a/Consultar Links Apostillas/Entrada.xlsx
+++ b/Consultar Links Apostillas/Entrada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\OneDrive\Escritorio\Automatizaciones-ApostillaColombia\Antecedentes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\OneDrive\Escritorio\Automatizaciones-ApostillaColombia\Consultar Links Apostillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1453150-27ED-4226-A745-DA8D90CD24BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2F9948-F332-4017-9ADC-3E8144693C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="2460" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,88 +33,89 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>CEDULA</t>
-  </si>
-  <si>
-    <t>FECHA_EXP</t>
-  </si>
-  <si>
-    <t>CODIGO</t>
-  </si>
-  <si>
-    <t>LINK</t>
-  </si>
-  <si>
     <t>OBSERVACIONES</t>
   </si>
   <si>
-    <t>BRIAN JOHAN CASTAÑO LOZANO</t>
-  </si>
-  <si>
-    <t>1115072206</t>
-  </si>
-  <si>
-    <t>ALIX VERONICA ESPINOSA TORRES</t>
-  </si>
-  <si>
-    <t>1093915412</t>
-  </si>
-  <si>
-    <t>DOUGLAS ANTONIO RENGIFO DIAZ</t>
-  </si>
-  <si>
-    <t>1144025784</t>
-  </si>
-  <si>
-    <t>YEINNY PAOLA RUDAS GUTIERREZ</t>
-  </si>
-  <si>
-    <t>1225092556</t>
-  </si>
-  <si>
-    <t>SCHENEIDER MAHECHA TRIANA</t>
-  </si>
-  <si>
-    <t>1070955418</t>
-  </si>
-  <si>
-    <t>MARTHA STELLA MORALES SANCHEZ</t>
-  </si>
-  <si>
-    <t>1073230817</t>
-  </si>
-  <si>
-    <t>LUIS JHONATAN VELASQUEZ MONTES</t>
-  </si>
-  <si>
-    <t>1151935587</t>
-  </si>
-  <si>
-    <t>KAMEL HASSAN GOMEZ HERNANDEZ</t>
-  </si>
-  <si>
-    <t>1115092664</t>
-  </si>
-  <si>
-    <t>La fecha de expedición de la cédula de ciudadanía no es válida.</t>
+    <t>ESTUDIANTE</t>
+  </si>
+  <si>
+    <t>COD. DIPLOMA</t>
+  </si>
+  <si>
+    <t>COD. NOTAS</t>
+  </si>
+  <si>
+    <t>COD. REGISTRO</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>RESPONDE</t>
+  </si>
+  <si>
+    <t>SOLICITA</t>
+  </si>
+  <si>
+    <t>ADICIONAL</t>
+  </si>
+  <si>
+    <t>PAOLA ANDREA LUNA HERNANDEZ</t>
+  </si>
+  <si>
+    <t>cesar</t>
+  </si>
+  <si>
+    <t>Maria Eugenia</t>
+  </si>
+  <si>
+    <t>GERMAN PAEZ RODRIGUEZ</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>SANDRA MILENA RIOS ZULUAGA</t>
+  </si>
+  <si>
+    <t>WILLIAM ANDRES VICUÑA MUÑOZ</t>
+  </si>
+  <si>
+    <t>PTE CODIGO</t>
+  </si>
+  <si>
+    <t>JULIETH FERNANDA VALENZUELA ALARCON</t>
+  </si>
+  <si>
+    <t>VENCIDO</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Diploma</t>
+  </si>
+  <si>
+    <t>Registro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,16 +128,48 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F8F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -159,24 +192,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -477,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C2" sqref="C2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,166 +616,209 @@
     <col min="5" max="5" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2">
-        <v>39472</v>
-      </c>
-      <c r="E2" s="4">
-        <v>52592623210</v>
+        <v>11</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="8">
+        <v>5259301181050</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="5">
+        <v>45896</v>
+      </c>
+      <c r="H2" s="6">
+        <v>165</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2">
-        <v>40925</v>
-      </c>
-      <c r="E3" s="4">
-        <v>525926181912512</v>
+        <v>14</v>
+      </c>
+      <c r="C3" s="10">
+        <v>5250000000000</v>
+      </c>
+      <c r="D3" s="11">
+        <v>525926229191323</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5">
+        <v>45897</v>
+      </c>
+      <c r="H3" s="6">
+        <v>110</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="14">
+        <v>52593020120155</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5">
+        <v>45897</v>
+      </c>
+      <c r="H4" s="6">
+        <v>110</v>
+      </c>
+      <c r="I4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2">
-        <v>39239</v>
-      </c>
-      <c r="E4" s="4">
-        <v>5259236422014</v>
+      <c r="J4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="11">
+        <v>52593014315122</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5">
+        <v>45897</v>
+      </c>
+      <c r="H5" s="6">
+        <v>165</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2">
-        <v>42894</v>
-      </c>
-      <c r="E5" s="4">
-        <v>52592615842015</v>
-      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2">
-        <v>39363</v>
-      </c>
-      <c r="E6" s="4">
-        <v>525926121910248</v>
+        <v>19</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="14">
+        <v>525930111920199</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5">
+        <v>45922</v>
+      </c>
+      <c r="H6" s="6">
+        <v>165</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2">
-        <v>38357</v>
-      </c>
-      <c r="E7" s="4">
-        <v>525926141015424</v>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="H7" s="6">
+        <v>715</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="2">
-        <v>41190</v>
-      </c>
-      <c r="E8" s="4">
-        <v>52592613138111</v>
-      </c>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2">
-        <v>42793</v>
-      </c>
-      <c r="G9" t="s">
-        <v>23</v>
-      </c>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://tramites.cancilleria.gov.co/apostillalegalizacion/consulta/documento.aspx?cod=A2ZJZE1413443101&amp;fecha=09/30/2025" xr:uid="{F7212A80-137C-44AF-AEDA-0A8F371811BF}"/>
+    <hyperlink ref="E2" r:id="rId2" display="https://tramites.cancilleria.gov.co/apostillalegalizacion/consulta/documento.aspx?cod=A2ZJZA13280741&amp;fecha=09/26/2025" xr:uid="{FAD21367-17F5-4833-8239-D32B466851FA}"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://tramites.cancilleria.gov.co/apostillalegalizacion/consulta/documento.aspx?cod=A2ZJZA13280741&amp;fecha=09/26/2025" xr:uid="{EC24EFEC-3437-46D7-8D81-176E8163EABD}"/>
+    <hyperlink ref="C5" r:id="rId4" display="https://tramites.cancilleria.gov.co/apostillalegalizacion/consulta/documento.aspx?cod=A2ZJZE141802071&amp;fecha=09/30/2025" xr:uid="{3B1F03FE-2581-4BFC-802A-7BC50572769C}"/>
+    <hyperlink ref="C6" r:id="rId5" display="https://tramites.cancilleria.gov.co/apostillalegalizacion/consulta/documento.aspx?cod=A2ZJZE141669071&amp;fecha=09/30/2025" xr:uid="{89931034-E81E-465B-BD0D-EBA0B66D4AAC}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>